<commit_message>
unsure what happened here but I'm committing anyway
</commit_message>
<xml_diff>
--- a/tests/integration_files/Test File 1.xlsx
+++ b/tests/integration_files/Test File 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loreal-my.sharepoint.com/personal/christopher_quartararo_loreal_com/Documents/Documents/Tools (Custom tooling)/Python/Coloshot Automation/tests/integration_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{21494157-99AD-44A5-9FF6-1CF1E57C3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A0003D4-E40D-440E-B0ED-E8D5DE03A275}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{21494157-99AD-44A5-9FF6-1CF1E57C3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3CCF9CC-05B5-4CD1-AFB1-28CC6EBF88EC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{12B5EF42-7A4F-4DFC-9639-A739315DF45A}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{12B5EF42-7A4F-4DFC-9639-A739315DF45A}"/>
   </bookViews>
   <sheets>
     <sheet name="Curve" sheetId="2" r:id="rId1"/>
@@ -588,9 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AF830D-796A-43D8-ABA3-099D05DF4783}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -600,13 +600,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB48ECE8-3221-4F66-9830-5B0B129F2CB4}">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -712,7 +716,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -744,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -776,7 +780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -808,7 +812,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -840,7 +844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -872,7 +876,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -904,7 +908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -936,7 +940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -968,7 +972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1096,7 +1100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1160,7 +1164,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -1192,7 +1196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Now adds file paths to report
</commit_message>
<xml_diff>
--- a/tests/integration_files/Test File 1.xlsx
+++ b/tests/integration_files/Test File 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loreal-my.sharepoint.com/personal/christopher_quartararo_loreal_com/Documents/Documents/Tools (Custom tooling)/Python/Coloshot Automation/tests/integration_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{21494157-99AD-44A5-9FF6-1CF1E57C3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3CCF9CC-05B5-4CD1-AFB1-28CC6EBF88EC}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{21494157-99AD-44A5-9FF6-1CF1E57C3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A914B8A2-733E-455B-94AC-14143BA1FAD7}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{12B5EF42-7A4F-4DFC-9639-A739315DF45A}"/>
+    <workbookView minimized="1" xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{12B5EF42-7A4F-4DFC-9639-A739315DF45A}"/>
   </bookViews>
   <sheets>
     <sheet name="Curve" sheetId="2" r:id="rId1"/>
@@ -601,13 +601,14 @@
   <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>